<commit_message>
Site updated: 2024-10-24 13:42:59
</commit_message>
<xml_diff>
--- a/files/生日策划-工作日志.xlsx
+++ b/files/生日策划-工作日志.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangmingjie/Desktop/研究生文件/2024/2024-12/lq生日/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangmingjie/Developer/website-info/source/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EDD968-E704-D74F-B8C6-266DF688A945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847393E-B43C-B149-A283-EF19BB3BB5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2600" yWindow="-19160" windowWidth="28240" windowHeight="17440" xr2:uid="{5840B6A6-0681-6743-9732-689998539898}"/>
+    <workbookView xWindow="4860" yWindow="-19000" windowWidth="28240" windowHeight="17440" xr2:uid="{5840B6A6-0681-6743-9732-689998539898}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>小王</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,6 +90,18 @@
   </si>
   <si>
     <t>9号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>现场工作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线上支持</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>紧急响应</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -130,12 +142,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -167,7 +197,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -177,16 +207,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -503,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DACB8B-0F90-564C-94EB-44E7D58DAF5C}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A9" sqref="A9:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -550,99 +583,97 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="A9" s="5"/>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="A10" s="6"/>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A11" s="7"/>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Site updated: 2024-10-24 14:34:32
</commit_message>
<xml_diff>
--- a/files/生日策划-工作日志.xlsx
+++ b/files/生日策划-工作日志.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangmingjie/Developer/website-info/source/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A847393E-B43C-B149-A283-EF19BB3BB5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1AC22E7-9147-2846-ADA5-D84D8FFAB279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4860" yWindow="-19000" windowWidth="28240" windowHeight="17440" xr2:uid="{5840B6A6-0681-6743-9732-689998539898}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +141,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -163,12 +170,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FFF8CBAD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,6 +198,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -219,8 +241,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,7 +561,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>